<commit_message>
ESP32 updates, better analysis formatting
</commit_message>
<xml_diff>
--- a/SDLowPowerLogs.xlsx
+++ b/SDLowPowerLogs.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaidica/Documents/Arduino/Neurotech Hub/SD Low Power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2923801B-5BDF-FC44-B0A9-8ECD412719A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3578830-436E-FB42-9D1A-B705A4547789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="5260" windowWidth="28040" windowHeight="17440" xr2:uid="{302C313D-8519-5945-A4BB-A4E7F74B0CFB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Adalogger M0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -488,9 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28114141-BB17-894E-8BBB-648411F9A015}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>